<commit_message>
Added io reading stuff and h2b parsing stuff
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manmeet Singh\Desktop\P&amp;PIV\Week 3\Assignments\The Level Renderer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manmeet Singh\Desktop\Project-And-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72ACA045-5FC2-464A-9EB9-B203409A5F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B3EE63-59BE-442C-8BA8-F2328CF2A6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="1380" windowWidth="21600" windowHeight="11295" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2039,7 +2039,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2066,8 +2066,8 @@
       <c r="B2" s="3">
         <v>0.02</v>
       </c>
-      <c r="C2" s="3">
-        <v>0</v>
+      <c r="C2" s="21">
+        <v>0.02</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2077,8 +2077,8 @@
       <c r="B3" s="3">
         <v>0.01</v>
       </c>
-      <c r="C3" s="3">
-        <v>0</v>
+      <c r="C3" s="21">
+        <v>0.01</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2088,8 +2088,8 @@
       <c r="B4" s="3">
         <v>0.05</v>
       </c>
-      <c r="C4" s="3">
-        <v>0</v>
+      <c r="C4" s="21">
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2099,8 +2099,8 @@
       <c r="B5" s="3">
         <v>0.01</v>
       </c>
-      <c r="C5" s="3">
-        <v>0</v>
+      <c r="C5" s="21">
+        <v>0.01</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2179,7 +2179,7 @@
       </c>
       <c r="C12" s="6">
         <f>SUM(C2:C11)</f>
-        <v>0.03</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2603,7 +2603,7 @@
       </c>
       <c r="C50" s="17">
         <f>MIN(SUM(C49,C44,C26,C12),100%)</f>
-        <v>0.05</v>
+        <v>0.13999999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the render issues, now can draw level no problem
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manmeet Singh\Desktop\Project-And-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B3EE63-59BE-442C-8BA8-F2328CF2A6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D4B3FC-1A47-4328-B69B-3DF3B124D1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -2039,7 +2039,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2110,8 +2110,8 @@
       <c r="B6" s="3">
         <v>0.03</v>
       </c>
-      <c r="C6" s="3">
-        <v>0</v>
+      <c r="C6" s="21">
+        <v>0.03</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2121,8 +2121,8 @@
       <c r="B7" s="3">
         <v>0.1</v>
       </c>
-      <c r="C7" s="3">
-        <v>0</v>
+      <c r="C7" s="21">
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2143,8 +2143,8 @@
       <c r="B9" s="3">
         <v>0.1</v>
       </c>
-      <c r="C9" s="3">
-        <v>0</v>
+      <c r="C9" s="21">
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2154,8 +2154,8 @@
       <c r="B10" s="3">
         <v>0.1</v>
       </c>
-      <c r="C10" s="3">
-        <v>0</v>
+      <c r="C10" s="21">
+        <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2165,8 +2165,8 @@
       <c r="B11" s="3">
         <v>0.05</v>
       </c>
-      <c r="C11" s="3">
-        <v>0</v>
+      <c r="C11" s="21">
+        <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2179,7 +2179,7 @@
       </c>
       <c r="C12" s="6">
         <f>SUM(C2:C11)</f>
-        <v>0.12</v>
+        <v>0.49999999999999994</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2603,7 +2603,7 @@
       </c>
       <c r="C50" s="17">
         <f>MIN(SUM(C49,C44,C26,C12),100%)</f>
-        <v>0.13999999999999999</v>
+        <v>0.51999999999999991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added file loading support
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manmeet Singh\Desktop\Project-And-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D4B3FC-1A47-4328-B69B-3DF3B124D1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8D8B05-9D74-46A7-BFDE-0C140DFD9695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -2039,7 +2039,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2200,8 +2200,8 @@
       <c r="B14" s="3">
         <v>0.11</v>
       </c>
-      <c r="C14" s="3">
-        <v>0</v>
+      <c r="C14" s="21">
+        <v>0.11</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2334,7 +2334,7 @@
       </c>
       <c r="C26" s="6">
         <f>MIN(SUM(C14:C25),33%)</f>
-        <v>0</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2603,7 +2603,7 @@
       </c>
       <c r="C50" s="17">
         <f>MIN(SUM(C49,C44,C26,C12),100%)</f>
-        <v>0.51999999999999991</v>
+        <v>0.62999999999999989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ability to read in Light Data from blender
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manmeet Singh\Desktop\Project-And-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8D8B05-9D74-46A7-BFDE-0C140DFD9695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827247CB-C890-4CAB-957A-CE7D4F6C3E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="3420" yWindow="1725" windowWidth="21600" windowHeight="11295" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2038,8 +2038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2211,8 +2211,8 @@
       <c r="B15" s="3">
         <v>0.11</v>
       </c>
-      <c r="C15" s="3">
-        <v>0</v>
+      <c r="C15" s="21">
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2334,7 +2334,7 @@
       </c>
       <c r="C26" s="6">
         <f>MIN(SUM(C14:C25),33%)</f>
-        <v>0.11</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2555,7 +2555,7 @@
         <v>0.02</v>
       </c>
       <c r="C46" s="3">
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2590,7 +2590,7 @@
       </c>
       <c r="C49" s="14">
         <f>SUM(C46:C48)</f>
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2603,7 +2603,7 @@
       </c>
       <c r="C50" s="17">
         <f>MIN(SUM(C49,C44,C26,C12),100%)</f>
-        <v>0.62999999999999989</v>
+        <v>0.72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Minimap and Game Music
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manmeet Singh\Desktop\Project-And-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827247CB-C890-4CAB-957A-CE7D4F6C3E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08DEE2F-2514-43A5-A147-480EE6697A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="1725" windowWidth="21600" windowHeight="11295" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -1267,7 +1267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -1414,6 +1414,9 @@
   </si>
   <si>
     <t>Make the camera Collide with your Level</t>
+  </si>
+  <si>
+    <t>I read in light info from .py and set everything accordingly… just don’t have multiple light support</t>
   </si>
 </sst>
 </file>
@@ -2036,10 +2039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2048,7 +2051,7 @@
     <col min="2" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -2059,7 +2062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2070,7 +2073,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2081,7 +2084,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>36</v>
       </c>
@@ -2092,7 +2095,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
@@ -2103,7 +2106,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2114,7 +2117,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -2125,7 +2128,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
@@ -2136,7 +2139,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>43</v>
       </c>
@@ -2147,7 +2150,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -2158,7 +2161,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -2169,7 +2172,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -2182,7 +2185,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -2193,7 +2196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>22</v>
       </c>
@@ -2204,7 +2207,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>41</v>
       </c>
@@ -2214,8 +2217,11 @@
       <c r="C15" s="21">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>40</v>
       </c>
@@ -2244,8 +2250,8 @@
       <c r="B18" s="3">
         <v>0.11</v>
       </c>
-      <c r="C18" s="3">
-        <v>0</v>
+      <c r="C18" s="21">
+        <v>0.11</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2334,7 +2340,7 @@
       </c>
       <c r="C26" s="6">
         <f>MIN(SUM(C14:C25),33%)</f>
-        <v>0.18</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2554,7 +2560,7 @@
       <c r="B46" s="3">
         <v>0.02</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="21">
         <v>0.02</v>
       </c>
     </row>
@@ -2603,7 +2609,7 @@
       </c>
       <c r="C50" s="17">
         <f>MIN(SUM(C49,C44,C26,C12),100%)</f>
-        <v>0.72</v>
+        <v>0.82999999999999985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>